<commit_message>
Ran line coverage/added tests; all lines covered
</commit_message>
<xml_diff>
--- a/graphTests.xlsx
+++ b/graphTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolemorris/morrinic/cs6015/assignment3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolemorris/cs6015assn4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83F17F68-FDFB-4642-8540-BAE08496D55E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021EE527-1BD6-2B48-BEC8-0BE7325B413C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{9F2D97F2-42F1-094A-A1E6-40474D1E2550}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="26520" windowHeight="16140" xr2:uid="{9F2D97F2-42F1-094A-A1E6-40474D1E2550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,13 +219,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -243,10 +243,10 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -273,6 +273,7 @@
         <c:axId val="675546112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1347,7 +1348,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1381,7 +1382,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -1395,10 +1396,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1409,10 +1410,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>10</v>

</xml_diff>